<commit_message>
cleaned the datas + 3rd figure and formatting
</commit_message>
<xml_diff>
--- a/dataset/Impfquotenmonitoring.xlsx
+++ b/dataset/Impfquotenmonitoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Pyt project\Dashboard-py\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\gitprojects\Dashboard-py\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBF048E-366C-4154-BA25-013BC59C53F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765283D5-4F81-4EB1-8141-ADFB55C7B4EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27660" yWindow="-1485" windowWidth="21600" windowHeight="11265" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Impfungen_proTag" sheetId="10" r:id="rId1"/>
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Gesamt</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Datum</t>
   </si>
@@ -142,7 +139,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -157,9 +154,6 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
@@ -503,35 +497,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926B42D2-7956-44E7-BD5B-5AF896796AC0}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>44192</v>
       </c>
@@ -545,7 +539,7 @@
         <v>23555</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>44193</v>
       </c>
@@ -559,7 +553,7 @@
         <v>18745</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>44194</v>
       </c>
@@ -573,7 +567,7 @@
         <v>42579</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>44195</v>
       </c>
@@ -587,7 +581,7 @@
         <v>57946</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>44196</v>
       </c>
@@ -601,7 +595,7 @@
         <v>38621</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>44197</v>
       </c>
@@ -615,7 +609,7 @@
         <v>24754</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>44198</v>
       </c>
@@ -629,7 +623,7 @@
         <v>51891</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>44199</v>
       </c>
@@ -643,7 +637,7 @@
         <v>24990</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>44200</v>
       </c>
@@ -657,7 +651,7 @@
         <v>48606</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>44201</v>
       </c>
@@ -671,7 +665,7 @@
         <v>52391</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>44202</v>
       </c>
@@ -685,7 +679,7 @@
         <v>58698</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>44203</v>
       </c>
@@ -699,7 +693,7 @@
         <v>58403</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>44204</v>
       </c>
@@ -713,7 +707,7 @@
         <v>60425</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>44205</v>
       </c>
@@ -727,7 +721,7 @@
         <v>57236</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <v>44206</v>
       </c>
@@ -741,7 +735,7 @@
         <v>33289</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>44207</v>
       </c>
@@ -755,7 +749,7 @@
         <v>65672</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <v>44208</v>
       </c>
@@ -769,7 +763,7 @@
         <v>82140</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <v>44209</v>
       </c>
@@ -783,7 +777,7 @@
         <v>99077</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>44210</v>
       </c>
@@ -797,7 +791,7 @@
         <v>100168</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
         <v>44211</v>
       </c>
@@ -811,7 +805,7 @@
         <v>92683</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
         <v>44212</v>
       </c>
@@ -825,7 +819,7 @@
         <v>57113</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
         <v>44213</v>
       </c>
@@ -839,7 +833,7 @@
         <v>44552</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <v>44214</v>
       </c>
@@ -853,7 +847,7 @@
         <v>74228</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
         <v>44215</v>
       </c>
@@ -867,7 +861,7 @@
         <v>95127</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
         <v>44216</v>
       </c>
@@ -881,7 +875,7 @@
         <v>128759</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>44217</v>
       </c>
@@ -895,7 +889,7 @@
         <v>96026</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
         <v>44218</v>
       </c>
@@ -909,7 +903,7 @@
         <v>115331</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="6">
         <v>44219</v>
       </c>
@@ -923,7 +917,7 @@
         <v>92599</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
         <v>44220</v>
       </c>
@@ -937,7 +931,7 @@
         <v>66100</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="6">
         <v>44221</v>
       </c>
@@ -951,7 +945,7 @@
         <v>97339</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
         <v>44222</v>
       </c>
@@ -965,7 +959,7 @@
         <v>102672</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="6">
         <v>44223</v>
       </c>
@@ -979,7 +973,7 @@
         <v>112992</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="6">
         <v>44224</v>
       </c>
@@ -993,7 +987,7 @@
         <v>100547</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
         <v>44225</v>
       </c>
@@ -1007,7 +1001,7 @@
         <v>109266</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="6">
         <v>44226</v>
       </c>
@@ -1021,7 +1015,7 @@
         <v>87283</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="6">
         <v>44227</v>
       </c>
@@ -1035,7 +1029,7 @@
         <v>62672</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="6">
         <v>44228</v>
       </c>
@@ -1049,7 +1043,7 @@
         <v>115626</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="6">
         <v>44229</v>
       </c>
@@ -1063,7 +1057,7 @@
         <v>127583</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="6">
         <v>44230</v>
       </c>
@@ -1077,7 +1071,7 @@
         <v>142360</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="6">
         <v>44231</v>
       </c>
@@ -1091,7 +1085,7 @@
         <v>135492</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="6">
         <v>44232</v>
       </c>
@@ -1105,7 +1099,7 @@
         <v>132037</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="6">
         <v>44233</v>
       </c>
@@ -1119,7 +1113,7 @@
         <v>103745</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="6">
         <v>44234</v>
       </c>
@@ -1133,7 +1127,7 @@
         <v>59398</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="6">
         <v>44235</v>
       </c>
@@ -1147,7 +1141,7 @@
         <v>107365</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="6">
         <v>44236</v>
       </c>
@@ -1161,7 +1155,7 @@
         <v>124699</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
         <v>44237</v>
       </c>
@@ -1175,7 +1169,7 @@
         <v>149166</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="6">
         <v>44238</v>
       </c>
@@ -1189,7 +1183,7 @@
         <v>143618</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="6">
         <v>44239</v>
       </c>
@@ -1203,7 +1197,7 @@
         <v>157760</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="6">
         <v>44240</v>
       </c>
@@ -1217,7 +1211,7 @@
         <v>109857</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="6">
         <v>44241</v>
       </c>
@@ -1231,7 +1225,7 @@
         <v>66763</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="6">
         <v>44242</v>
       </c>
@@ -1245,7 +1239,7 @@
         <v>126776</v>
       </c>
     </row>
-    <row r="53" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="6">
         <v>44243</v>
       </c>
@@ -1259,7 +1253,7 @@
         <v>136119</v>
       </c>
     </row>
-    <row r="54" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="6">
         <v>44244</v>
       </c>
@@ -1273,7 +1267,7 @@
         <v>148915</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="6">
         <v>44245</v>
       </c>
@@ -1287,7 +1281,7 @@
         <v>144951</v>
       </c>
     </row>
-    <row r="56" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="6">
         <v>44246</v>
       </c>
@@ -1301,7 +1295,7 @@
         <v>150036</v>
       </c>
     </row>
-    <row r="57" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="6">
         <v>44247</v>
       </c>
@@ -1315,7 +1309,7 @@
         <v>112498</v>
       </c>
     </row>
-    <row r="58" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="6">
         <v>44248</v>
       </c>
@@ -1329,7 +1323,7 @@
         <v>85593</v>
       </c>
     </row>
-    <row r="59" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="6">
         <v>44249</v>
       </c>
@@ -1343,7 +1337,7 @@
         <v>151701</v>
       </c>
     </row>
-    <row r="60" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="6">
         <v>44250</v>
       </c>
@@ -1357,7 +1351,7 @@
         <v>159068</v>
       </c>
     </row>
-    <row r="61" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="6">
         <v>44251</v>
       </c>
@@ -1371,7 +1365,7 @@
         <v>173410</v>
       </c>
     </row>
-    <row r="62" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="6">
         <v>44252</v>
       </c>
@@ -1385,7 +1379,7 @@
         <v>177768</v>
       </c>
     </row>
-    <row r="63" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="6">
         <v>44253</v>
       </c>
@@ -1399,63 +1393,63 @@
         <v>190234</v>
       </c>
     </row>
-    <row r="64" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="6">
         <v>44254</v>
       </c>
-      <c r="B64" s="8">
+      <c r="B64" s="7">
         <v>106896</v>
       </c>
-      <c r="C64" s="8">
+      <c r="C64" s="7">
         <v>38515</v>
       </c>
-      <c r="D64" s="8">
+      <c r="D64" s="7">
         <v>145411</v>
       </c>
     </row>
-    <row r="65" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="6">
         <v>44255</v>
       </c>
-      <c r="B65" s="8">
+      <c r="B65" s="7">
         <v>85568</v>
       </c>
-      <c r="C65" s="8">
+      <c r="C65" s="7">
         <v>27653</v>
       </c>
-      <c r="D65" s="8">
+      <c r="D65" s="7">
         <v>113221</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="6">
         <v>44256</v>
       </c>
-      <c r="B66" s="8">
+      <c r="B66" s="7">
         <v>138451</v>
       </c>
-      <c r="C66" s="8">
+      <c r="C66" s="7">
         <v>49291</v>
       </c>
-      <c r="D66" s="8">
+      <c r="D66" s="7">
         <v>187742</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="6">
         <v>44257</v>
       </c>
-      <c r="B67" s="8">
+      <c r="B67" s="7">
         <v>153763</v>
       </c>
-      <c r="C67" s="8">
+      <c r="C67" s="7">
         <v>54331</v>
       </c>
-      <c r="D67" s="8">
+      <c r="D67" s="7">
         <v>208094</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="6">
         <v>44258</v>
       </c>
@@ -1467,23 +1461,6 @@
       </c>
       <c r="D68">
         <v>191692</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B69" s="3">
-        <f>SUM(B2:B68)</f>
-        <v>4541389</v>
-      </c>
-      <c r="C69" s="3">
-        <f>SUM(C2:C68)</f>
-        <v>2271784</v>
-      </c>
-      <c r="D69" s="3">
-        <f>SUM(D2:D68)</f>
-        <v>6813173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>